<commit_message>
Alta de Vistas y actualización de Controlador
</commit_message>
<xml_diff>
--- a/Documentos/Plan de Trabajo ASN v6.xlsx
+++ b/Documentos/Plan de Trabajo ASN v6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desarrollo\ASN\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8435E425-AD05-4DB7-9751-D93DC022B00F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E54D88E-4FDF-4949-88A8-CB167A40711F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="671" firstSheet="2" activeTab="4" xr2:uid="{E673171D-683B-4146-8516-79FB6088E25E}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="324">
   <si>
     <t>Artefacto</t>
   </si>
@@ -1504,6 +1504,51 @@
   </si>
   <si>
     <t>Motivos</t>
+  </si>
+  <si>
+    <t>Solicitud</t>
+  </si>
+  <si>
+    <t>Seguridad</t>
+  </si>
+  <si>
+    <t>CoordinadoresNomina</t>
+  </si>
+  <si>
+    <t>Captura</t>
+  </si>
+  <si>
+    <t>CargaDocumento</t>
+  </si>
+  <si>
+    <t>CargaMasiva</t>
+  </si>
+  <si>
+    <t>Nomina</t>
+  </si>
+  <si>
+    <t>Periodos</t>
+  </si>
+  <si>
+    <t>Administracion</t>
+  </si>
+  <si>
+    <t>Notificaciones</t>
+  </si>
+  <si>
+    <t>GeneracionEXCEL</t>
+  </si>
+  <si>
+    <t>Reporte</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Auditoria</t>
+  </si>
+  <si>
+    <t>CierreMovimientos</t>
   </si>
 </sst>
 </file>
@@ -3955,7 +4000,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3964,7 +4009,10 @@
     <col min="2" max="2" width="5.140625" style="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="88.140625" style="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="11.140625" style="19"/>
+    <col min="5" max="5" width="11.140625" style="19"/>
+    <col min="6" max="6" width="19.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="19"/>
     <col min="9" max="9" width="47.28515625" style="19" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="11.140625" style="19"/>
   </cols>
@@ -4053,6 +4101,9 @@
       <c r="D5" s="19">
         <v>1</v>
       </c>
+      <c r="F5" s="19" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
@@ -4067,6 +4118,12 @@
       <c r="D6" s="19" t="s">
         <v>257</v>
       </c>
+      <c r="F6" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
@@ -4101,6 +4158,12 @@
       <c r="D8" s="19" t="s">
         <v>257</v>
       </c>
+      <c r="F8" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
@@ -4115,6 +4178,12 @@
       <c r="D9" s="19">
         <v>1</v>
       </c>
+      <c r="F9" s="19" t="s">
+        <v>310</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
@@ -4129,6 +4198,12 @@
       <c r="D10" s="19">
         <v>3</v>
       </c>
+      <c r="F10" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
@@ -4143,6 +4218,12 @@
       <c r="D11" s="19">
         <v>1</v>
       </c>
+      <c r="F11" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
@@ -4157,6 +4238,12 @@
       <c r="D12" s="19">
         <v>2</v>
       </c>
+      <c r="F12" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
@@ -4185,6 +4272,12 @@
       <c r="D14" s="19">
         <v>1</v>
       </c>
+      <c r="F14" s="19" t="s">
+        <v>315</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
@@ -4199,6 +4292,12 @@
       <c r="D15" s="19">
         <v>1</v>
       </c>
+      <c r="F15" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
@@ -4213,8 +4312,14 @@
       <c r="D16" s="19" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F16" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>256</v>
       </c>
@@ -4227,8 +4332,14 @@
       <c r="D17" s="19">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F17" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>256</v>
       </c>
@@ -4241,8 +4352,14 @@
       <c r="D18" s="19">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F18" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>256</v>
       </c>
@@ -4256,7 +4373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>256</v>
       </c>
@@ -4270,7 +4387,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>256</v>
       </c>
@@ -4283,8 +4400,14 @@
       <c r="D21" s="19">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F21" s="19" t="s">
+        <v>320</v>
+      </c>
+      <c r="G21" s="19" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>256</v>
       </c>
@@ -4297,8 +4420,14 @@
       <c r="D22" s="19">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F22" s="19" t="s">
+        <v>320</v>
+      </c>
+      <c r="G22" s="19" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>256</v>
       </c>
@@ -4311,8 +4440,14 @@
       <c r="D23" s="19">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F23" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="G23" s="19" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C25" s="20" t="s">
         <v>259</v>
       </c>

</xml_diff>